<commit_message>
add spec for excel parser
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/test.xlsx
+++ b/spec/fixtures/files/test.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/radin/workspaces/projects/mobiles/eoc/eoc-web/spec/fixtures/files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/borey/project/eoc-web/spec/fixtures/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B107DFC-2B41-B841-AAF5-E1228380105F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE737C36-9FDA-F841-8349-B1BE57350105}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="10260" xr2:uid="{37A80561-3808-4A4B-9B76-1E15D49631FE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="1" xr2:uid="{37A80561-3808-4A4B-9B76-1E15D49631FE}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="categories" sheetId="1" r:id="rId1"/>
+    <sheet name="sops" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,52 +26,64 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Tags</t>
-  </si>
-  <si>
-    <t>File</t>
-  </si>
-  <si>
-    <t>Malaria</t>
-  </si>
-  <si>
-    <t>malaria Cambodia phnom_penh</t>
-  </si>
-  <si>
-    <t>HIV/AIDS</t>
-  </si>
-  <si>
-    <t>AIDS female_prostitutes drugs HIV illegal</t>
-  </si>
-  <si>
-    <t>Dengue Fever</t>
-  </si>
-  <si>
-    <t>dengue mosquitos rainy_season cambodia</t>
-  </si>
-  <si>
-    <t>Tuberculosis</t>
-  </si>
-  <si>
-    <t>tuberculosis Cambodia airborne_infection lungs</t>
-  </si>
-  <si>
-    <t>AnimalFarm.pdf</t>
-  </si>
-  <si>
-    <t>Document_type</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+  <si>
+    <t>parent</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>root cat</t>
+  </si>
+  <si>
+    <t>cat 1</t>
+  </si>
+  <si>
+    <t>cat 1.1</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>file</t>
+  </si>
+  <si>
+    <t>tags</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Hepatitis A</t>
+  </si>
+  <si>
+    <t>hepatitis-a high-danger</t>
+  </si>
+  <si>
+    <t>cat 2</t>
+  </si>
+  <si>
+    <t>Hepatitis A usually does not …</t>
+  </si>
+  <si>
+    <t>Acute.pdf</t>
+  </si>
+  <si>
+    <t>Animal.pdf</t>
+  </si>
+  <si>
+    <t>Animal</t>
+  </si>
+  <si>
+    <t>nothing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -92,15 +105,36 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="2" tint="-0.89999084444715716"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="16"/>
-      <color theme="1"/>
-      <name val="Calibri (Body)"/>
+      <sz val="14.4"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -119,34 +153,21 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -463,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0C1111-BDB8-1140-BC2E-CF80A0B90436}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.5" defaultRowHeight="21"/>
@@ -476,69 +497,105 @@
     <col min="5" max="16384" width="25.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="3" customFormat="1">
+    <row r="1" spans="1:2" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C97548-00FB-3C43-BD05-34DC078AF3CA}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="19">
       <c r="A1" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="18">
+      <c r="A2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="5" t="s">
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1</v>
-      </c>
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>